<commit_message>
zaw - testing - manage user - commit
</commit_message>
<xml_diff>
--- a/documentation/04_テスト/01_単体テスト/Backend/01_テスト仕様書/プロフィールAPI＿テスト仕様書.xlsx
+++ b/documentation/04_テスト/01_単体テスト/Backend/01_テスト仕様書/プロフィールAPI＿テスト仕様書.xlsx
@@ -14,8 +14,8 @@
   <definedNames>
     <definedName name="_xlnm.Print_Titles" localSheetId="2">エビデンス!#REF!</definedName>
     <definedName name="_xlnm.Print_Titles" localSheetId="1">'基本情報（従業員）'!$1:$4</definedName>
-    <definedName name="_xlnm.Print_Area" localSheetId="2">エビデンス!$A$1:$AK$140</definedName>
-    <definedName name="_xlnm.Print_Area" localSheetId="1">'基本情報（従業員）'!$A$1:$BJ$8</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="2">エビデンス!$A$1:$AK$173</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="1">'基本情報（従業員）'!$A$1:$BJ$9</definedName>
   </definedNames>
   <calcPr calcId="144525"/>
 </workbook>
@@ -71,7 +71,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="69" uniqueCount="38">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="80" uniqueCount="42">
   <si>
     <t>単体テスト仕様書</t>
   </si>
@@ -191,6 +191,19 @@
     <t>1．レスポンスステータスが４００であること</t>
   </si>
   <si>
+    <t>02_015_005</t>
+  </si>
+  <si>
+    <t>一覧</t>
+  </si>
+  <si>
+    <t>1．ユーザIDが存在すること</t>
+  </si>
+  <si>
+    <t>1．レスポンスステータスが２００であること
+2．レスポンスバディーにユーザーデータが返すこと</t>
+  </si>
+  <si>
     <t>リクエスト</t>
   </si>
   <si>
@@ -202,9 +215,9 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="5">
+    <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
     <numFmt numFmtId="176" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
     <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
     <numFmt numFmtId="177" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
     <numFmt numFmtId="178" formatCode="m/d"/>
   </numFmts>
@@ -281,9 +294,8 @@
       <charset val="128"/>
     </font>
     <font>
-      <u/>
       <sz val="11"/>
-      <color rgb="FF0000FF"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -298,7 +310,15 @@
     <font>
       <b/>
       <sz val="11"/>
-      <color theme="1"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -312,7 +332,7 @@
     </font>
     <font>
       <sz val="11"/>
-      <color theme="1"/>
+      <color rgb="FF9C0006"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -323,6 +343,51 @@
       <color theme="3"/>
       <name val="Calibri"/>
       <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF0000FF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="15"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -343,6 +408,14 @@
     </font>
     <font>
       <b/>
+      <sz val="18"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
       <sz val="13"/>
       <color theme="3"/>
       <name val="Calibri"/>
@@ -350,46 +423,9 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
       <sz val="11"/>
-      <color rgb="FFFF0000"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="18"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="15"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C0006"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -402,31 +438,8 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
       <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
+      <color rgb="FFFF0000"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -458,7 +471,31 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -470,7 +507,73 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="8"/>
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -482,25 +585,31 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
+        <fgColor rgb="FFA5A5A5"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
+        <fgColor theme="7"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
+        <fgColor theme="8"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -512,13 +621,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
+        <fgColor rgb="FFC6EFCE"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -530,7 +633,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
+        <fgColor theme="8" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -548,97 +651,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -905,65 +918,6 @@
       <top/>
       <bottom style="medium">
         <color auto="1"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color theme="4"/>
-      </top>
-      <bottom style="double">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="double">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="double">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="double">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="double">
-        <color rgb="FF3F3F3F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color rgb="FFB2B2B2"/>
-      </left>
-      <right style="thin">
-        <color rgb="FFB2B2B2"/>
-      </right>
-      <top style="thin">
-        <color rgb="FFB2B2B2"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FFB2B2B2"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
       </bottom>
       <diagonal/>
     </border>
@@ -1001,8 +955,67 @@
       <left/>
       <right/>
       <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
       <bottom style="double">
         <color rgb="FFFF8001"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="double">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="double">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="double">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="double">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FFB2B2B2"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFB2B2B2"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFB2B2B2"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFB2B2B2"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="double">
+        <color theme="4"/>
       </bottom>
       <diagonal/>
     </border>
@@ -1011,148 +1024,148 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="176" fontId="14" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="177" fontId="14" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="42" fontId="14" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="44" fontId="14" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="14" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="11" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="176" fontId="15" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="177" fontId="15" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="42" fontId="15" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="15" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="15" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="23" borderId="27" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="27" fillId="0" borderId="26" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="28" borderId="28" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="30" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="26" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="24" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="11" borderId="23" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="24" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="12" borderId="25" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="24" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="26" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="19" borderId="27" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="26" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="27" fillId="22" borderId="28" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="28" fillId="22" borderId="27" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="29" fillId="0" borderId="29" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="22" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="30" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="19" fillId="11" borderId="22" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="6" borderId="23" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="6" borderId="22" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="25" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="28" fillId="0" borderId="29" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="12" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="11" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="12" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="11" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
@@ -1939,6 +1952,82 @@
     </xdr:sp>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>9525</xdr:colOff>
+      <xdr:row>146</xdr:row>
+      <xdr:rowOff>9525</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>18</xdr:col>
+      <xdr:colOff>400050</xdr:colOff>
+      <xdr:row>169</xdr:row>
+      <xdr:rowOff>139700</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="10" name="Picture 9" descr="02_15_005_get_User_Data_request"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip r:embed="rId9"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="1743075" y="29769435"/>
+          <a:ext cx="9058275" cy="4818380"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>20</xdr:col>
+      <xdr:colOff>9525</xdr:colOff>
+      <xdr:row>146</xdr:row>
+      <xdr:rowOff>9525</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>35</xdr:col>
+      <xdr:colOff>266700</xdr:colOff>
+      <xdr:row>168</xdr:row>
+      <xdr:rowOff>5715</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="12" name="Picture 11" descr="02_015_005_get_User_Data_response"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip r:embed="rId10"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="11566525" y="29769435"/>
+          <a:ext cx="8924925" cy="4480560"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
 </xdr:wsDr>
 </file>
 
@@ -2398,7 +2487,7 @@
     <sheetView view="pageBreakPreview" zoomScaleNormal="130" workbookViewId="0">
       <pane ySplit="4" topLeftCell="A5" activePane="bottomLeft" state="frozen"/>
       <selection/>
-      <selection pane="bottomLeft" activeCell="J7" sqref="J7:N7"/>
+      <selection pane="bottomLeft" activeCell="BD9" sqref="BD9:BE9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.66666666666667" defaultRowHeight="16.05" customHeight="1"/>
@@ -2884,12 +2973,12 @@
       <c r="BM7" s="63"/>
     </row>
     <row r="8" ht="74.95" customHeight="1" spans="1:62">
-      <c r="A8" s="19" t="s">
+      <c r="A8" s="21" t="s">
         <v>33</v>
       </c>
-      <c r="B8" s="19"/>
-      <c r="C8" s="19"/>
-      <c r="D8" s="19"/>
+      <c r="B8" s="21"/>
+      <c r="C8" s="21"/>
+      <c r="D8" s="21"/>
       <c r="E8" s="22" t="s">
         <v>22</v>
       </c>
@@ -2911,40 +3000,40 @@
       <c r="Q8" s="22"/>
       <c r="R8" s="22"/>
       <c r="S8" s="22"/>
-      <c r="T8" s="20" t="s">
+      <c r="T8" s="22" t="s">
         <v>34</v>
       </c>
-      <c r="U8" s="20"/>
-      <c r="V8" s="20"/>
-      <c r="W8" s="20"/>
-      <c r="X8" s="20"/>
-      <c r="Y8" s="20"/>
-      <c r="Z8" s="20"/>
-      <c r="AA8" s="20"/>
-      <c r="AB8" s="20"/>
-      <c r="AC8" s="20"/>
-      <c r="AD8" s="20"/>
-      <c r="AE8" s="20"/>
-      <c r="AF8" s="20"/>
-      <c r="AG8" s="20"/>
-      <c r="AH8" s="20"/>
-      <c r="AI8" s="20" t="s">
+      <c r="U8" s="22"/>
+      <c r="V8" s="22"/>
+      <c r="W8" s="22"/>
+      <c r="X8" s="22"/>
+      <c r="Y8" s="22"/>
+      <c r="Z8" s="22"/>
+      <c r="AA8" s="22"/>
+      <c r="AB8" s="22"/>
+      <c r="AC8" s="22"/>
+      <c r="AD8" s="22"/>
+      <c r="AE8" s="22"/>
+      <c r="AF8" s="22"/>
+      <c r="AG8" s="22"/>
+      <c r="AH8" s="22"/>
+      <c r="AI8" s="22" t="s">
         <v>35</v>
       </c>
-      <c r="AJ8" s="20"/>
-      <c r="AK8" s="20"/>
-      <c r="AL8" s="20"/>
-      <c r="AM8" s="20"/>
-      <c r="AN8" s="20"/>
-      <c r="AO8" s="20"/>
-      <c r="AP8" s="20"/>
-      <c r="AQ8" s="20"/>
-      <c r="AR8" s="20"/>
-      <c r="AS8" s="20"/>
-      <c r="AT8" s="20"/>
-      <c r="AU8" s="20"/>
-      <c r="AV8" s="20"/>
-      <c r="AW8" s="20"/>
+      <c r="AJ8" s="22"/>
+      <c r="AK8" s="22"/>
+      <c r="AL8" s="22"/>
+      <c r="AM8" s="22"/>
+      <c r="AN8" s="22"/>
+      <c r="AO8" s="22"/>
+      <c r="AP8" s="22"/>
+      <c r="AQ8" s="22"/>
+      <c r="AR8" s="22"/>
+      <c r="AS8" s="22"/>
+      <c r="AT8" s="22"/>
+      <c r="AU8" s="22"/>
+      <c r="AV8" s="22"/>
+      <c r="AW8" s="22"/>
       <c r="AX8" s="53" t="s">
         <v>8</v>
       </c>
@@ -2959,75 +3048,93 @@
         <v>27</v>
       </c>
       <c r="BE8" s="21"/>
-      <c r="BF8" s="19"/>
-      <c r="BG8" s="19"/>
-      <c r="BH8" s="19"/>
-      <c r="BI8" s="52"/>
-      <c r="BJ8" s="52"/>
+      <c r="BF8" s="21"/>
+      <c r="BG8" s="21"/>
+      <c r="BH8" s="21"/>
+      <c r="BI8" s="54"/>
+      <c r="BJ8" s="54"/>
     </row>
     <row r="9" ht="74.95" customHeight="1" spans="1:62">
-      <c r="A9" s="23"/>
-      <c r="B9" s="23"/>
-      <c r="C9" s="23"/>
-      <c r="D9" s="23"/>
-      <c r="E9" s="24"/>
-      <c r="F9" s="24"/>
-      <c r="G9" s="24"/>
-      <c r="H9" s="24"/>
-      <c r="I9" s="24"/>
-      <c r="J9" s="24"/>
-      <c r="K9" s="24"/>
-      <c r="L9" s="24"/>
-      <c r="M9" s="24"/>
-      <c r="N9" s="24"/>
-      <c r="O9" s="24"/>
-      <c r="P9" s="24"/>
-      <c r="Q9" s="24"/>
-      <c r="R9" s="24"/>
-      <c r="S9" s="24"/>
-      <c r="T9" s="24"/>
-      <c r="U9" s="24"/>
-      <c r="V9" s="24"/>
-      <c r="W9" s="24"/>
-      <c r="X9" s="24"/>
-      <c r="Y9" s="24"/>
-      <c r="Z9" s="24"/>
-      <c r="AA9" s="24"/>
-      <c r="AB9" s="24"/>
-      <c r="AC9" s="24"/>
-      <c r="AD9" s="24"/>
-      <c r="AE9" s="24"/>
-      <c r="AF9" s="24"/>
-      <c r="AG9" s="24"/>
-      <c r="AH9" s="24"/>
-      <c r="AI9" s="24"/>
-      <c r="AJ9" s="24"/>
-      <c r="AK9" s="24"/>
-      <c r="AL9" s="24"/>
-      <c r="AM9" s="24"/>
-      <c r="AN9" s="24"/>
-      <c r="AO9" s="24"/>
-      <c r="AP9" s="24"/>
-      <c r="AQ9" s="24"/>
-      <c r="AR9" s="24"/>
-      <c r="AS9" s="24"/>
-      <c r="AT9" s="24"/>
-      <c r="AU9" s="24"/>
-      <c r="AV9" s="24"/>
-      <c r="AW9" s="24"/>
-      <c r="AX9" s="55"/>
-      <c r="AY9" s="55"/>
-      <c r="AZ9" s="55"/>
-      <c r="BA9" s="56"/>
-      <c r="BB9" s="56"/>
-      <c r="BC9" s="56"/>
-      <c r="BD9" s="23"/>
-      <c r="BE9" s="23"/>
-      <c r="BF9" s="23"/>
-      <c r="BG9" s="23"/>
-      <c r="BH9" s="23"/>
-      <c r="BI9" s="56"/>
-      <c r="BJ9" s="56"/>
+      <c r="A9" s="19" t="s">
+        <v>36</v>
+      </c>
+      <c r="B9" s="19"/>
+      <c r="C9" s="19"/>
+      <c r="D9" s="19"/>
+      <c r="E9" s="22" t="s">
+        <v>22</v>
+      </c>
+      <c r="F9" s="22"/>
+      <c r="G9" s="22"/>
+      <c r="H9" s="22"/>
+      <c r="I9" s="22"/>
+      <c r="J9" s="22" t="s">
+        <v>23</v>
+      </c>
+      <c r="K9" s="22"/>
+      <c r="L9" s="22"/>
+      <c r="M9" s="22"/>
+      <c r="N9" s="22"/>
+      <c r="O9" s="20" t="s">
+        <v>37</v>
+      </c>
+      <c r="P9" s="20"/>
+      <c r="Q9" s="20"/>
+      <c r="R9" s="20"/>
+      <c r="S9" s="20"/>
+      <c r="T9" s="20" t="s">
+        <v>38</v>
+      </c>
+      <c r="U9" s="20"/>
+      <c r="V9" s="20"/>
+      <c r="W9" s="20"/>
+      <c r="X9" s="20"/>
+      <c r="Y9" s="20"/>
+      <c r="Z9" s="20"/>
+      <c r="AA9" s="20"/>
+      <c r="AB9" s="20"/>
+      <c r="AC9" s="20"/>
+      <c r="AD9" s="20"/>
+      <c r="AE9" s="20"/>
+      <c r="AF9" s="20"/>
+      <c r="AG9" s="20"/>
+      <c r="AH9" s="20"/>
+      <c r="AI9" s="20" t="s">
+        <v>39</v>
+      </c>
+      <c r="AJ9" s="20"/>
+      <c r="AK9" s="20"/>
+      <c r="AL9" s="20"/>
+      <c r="AM9" s="20"/>
+      <c r="AN9" s="20"/>
+      <c r="AO9" s="20"/>
+      <c r="AP9" s="20"/>
+      <c r="AQ9" s="20"/>
+      <c r="AR9" s="20"/>
+      <c r="AS9" s="20"/>
+      <c r="AT9" s="20"/>
+      <c r="AU9" s="20"/>
+      <c r="AV9" s="20"/>
+      <c r="AW9" s="20"/>
+      <c r="AX9" s="53" t="s">
+        <v>8</v>
+      </c>
+      <c r="AY9" s="53"/>
+      <c r="AZ9" s="53"/>
+      <c r="BA9" s="54">
+        <v>44931</v>
+      </c>
+      <c r="BB9" s="54"/>
+      <c r="BC9" s="54"/>
+      <c r="BD9" s="21" t="s">
+        <v>27</v>
+      </c>
+      <c r="BE9" s="21"/>
+      <c r="BF9" s="19"/>
+      <c r="BG9" s="19"/>
+      <c r="BH9" s="19"/>
+      <c r="BI9" s="52"/>
+      <c r="BJ9" s="52"/>
     </row>
     <row r="10" ht="74.95" customHeight="1" spans="1:62">
       <c r="A10" s="23"/>
@@ -4626,9 +4733,9 @@
   <dimension ref="B3:BN171"/>
   <sheetViews>
     <sheetView tabSelected="1" view="pageBreakPreview" zoomScale="60" zoomScaleNormal="70" topLeftCell="B1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A104" activePane="bottomLeft" state="frozen"/>
+      <pane ySplit="1" topLeftCell="A113" activePane="bottomLeft" state="frozen"/>
       <selection/>
-      <selection pane="bottomLeft" activeCell="U130" sqref="U130"/>
+      <selection pane="bottomLeft" activeCell="W135" sqref="W135"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.66666666666667" defaultRowHeight="16.05" customHeight="1"/>
@@ -4692,12 +4799,12 @@
     </row>
     <row r="6" customHeight="1" spans="4:23">
       <c r="D6" s="4" t="s">
-        <v>36</v>
+        <v>40</v>
       </c>
       <c r="E6" s="4"/>
       <c r="F6" s="4"/>
       <c r="U6" s="9" t="s">
-        <v>37</v>
+        <v>41</v>
       </c>
       <c r="V6" s="9"/>
       <c r="W6" s="9"/>
@@ -4818,7 +4925,7 @@
       <c r="B43" s="8"/>
       <c r="C43" s="7"/>
       <c r="D43" s="4" t="s">
-        <v>36</v>
+        <v>40</v>
       </c>
       <c r="E43" s="4"/>
       <c r="F43" s="4"/>
@@ -4837,7 +4944,7 @@
       <c r="S43" s="7"/>
       <c r="T43" s="7"/>
       <c r="U43" s="9" t="s">
-        <v>37</v>
+        <v>41</v>
       </c>
       <c r="V43" s="9"/>
       <c r="W43" s="9"/>
@@ -5002,7 +5109,7 @@
       <c r="B75" s="8"/>
       <c r="C75" s="7"/>
       <c r="D75" s="4" t="s">
-        <v>36</v>
+        <v>40</v>
       </c>
       <c r="E75" s="4"/>
       <c r="F75" s="4"/>
@@ -5021,7 +5128,7 @@
       <c r="S75" s="7"/>
       <c r="T75" s="7"/>
       <c r="U75" s="9" t="s">
-        <v>37</v>
+        <v>41</v>
       </c>
       <c r="V75" s="9"/>
       <c r="W75" s="9"/>
@@ -5123,7 +5230,7 @@
       <c r="B109" s="8"/>
       <c r="C109" s="7"/>
       <c r="D109" s="4" t="s">
-        <v>36</v>
+        <v>40</v>
       </c>
       <c r="E109" s="4"/>
       <c r="F109" s="4"/>
@@ -5142,7 +5249,7 @@
       <c r="S109" s="7"/>
       <c r="T109" s="7"/>
       <c r="U109" s="9" t="s">
-        <v>37</v>
+        <v>41</v>
       </c>
       <c r="V109" s="9"/>
       <c r="W109" s="9"/>
@@ -5182,10 +5289,17 @@
       <c r="C140" s="7"/>
       <c r="D140" s="7"/>
     </row>
+    <row r="141" customHeight="1" spans="3:5">
+      <c r="C141" s="4" t="s">
+        <v>36</v>
+      </c>
+      <c r="D141" s="4"/>
+      <c r="E141" s="4"/>
+    </row>
     <row r="142" customHeight="1" spans="3:21">
-      <c r="C142" s="7"/>
-      <c r="D142" s="7"/>
-      <c r="E142" s="7"/>
+      <c r="C142" s="4"/>
+      <c r="D142" s="4"/>
+      <c r="E142" s="4"/>
       <c r="S142" s="7"/>
       <c r="T142" s="7"/>
       <c r="U142" s="7"/>
@@ -5198,6 +5312,26 @@
       <c r="T143" s="7"/>
       <c r="U143" s="7"/>
     </row>
+    <row r="144" customHeight="1" spans="4:23">
+      <c r="D144" s="4" t="s">
+        <v>40</v>
+      </c>
+      <c r="E144" s="4"/>
+      <c r="F144" s="4"/>
+      <c r="U144" s="9" t="s">
+        <v>41</v>
+      </c>
+      <c r="V144" s="9"/>
+      <c r="W144" s="9"/>
+    </row>
+    <row r="145" customHeight="1" spans="4:23">
+      <c r="D145" s="4"/>
+      <c r="E145" s="4"/>
+      <c r="F145" s="4"/>
+      <c r="U145" s="9"/>
+      <c r="V145" s="9"/>
+      <c r="W145" s="9"/>
+    </row>
     <row r="167" customHeight="1" spans="2:4">
       <c r="B167" s="7"/>
       <c r="C167" s="7"/>
@@ -5225,7 +5359,7 @@
       <c r="V171" s="7"/>
     </row>
   </sheetData>
-  <mergeCells count="13">
+  <mergeCells count="16">
     <mergeCell ref="C63:I64"/>
     <mergeCell ref="C3:E4"/>
     <mergeCell ref="D6:F7"/>
@@ -5239,18 +5373,20 @@
     <mergeCell ref="C106:E107"/>
     <mergeCell ref="D109:F110"/>
     <mergeCell ref="U109:W110"/>
+    <mergeCell ref="C141:E142"/>
+    <mergeCell ref="D144:F145"/>
+    <mergeCell ref="U144:W145"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" scale="41" orientation="landscape"/>
+  <pageSetup paperSize="9" scale="39" orientation="landscape"/>
   <headerFooter>
     <oddFooter>&amp;C&amp;P/&amp;N</oddFooter>
   </headerFooter>
-  <rowBreaks count="5" manualBreakCount="5">
+  <rowBreaks count="4" manualBreakCount="4">
     <brk id="37" max="16383" man="1"/>
     <brk id="70" max="16383" man="1"/>
     <brk id="104" max="16383" man="1"/>
-    <brk id="140" max="16383" man="1"/>
-    <brk id="165" max="35" man="1"/>
+    <brk id="139" max="36" man="1"/>
   </rowBreaks>
   <drawing r:id="rId1"/>
 </worksheet>

</xml_diff>